<commit_message>
Agregados de detalle en los resultados
</commit_message>
<xml_diff>
--- a/3.Outputs/3.2.Results/ASPL_CC_Q.xlsx
+++ b/3.Outputs/3.2.Results/ASPL_CC_Q.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03da0cbcfcedef2e/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eze\OneDrive\Escritorio\mainScriptNeuro\3.Outputs\3.2.Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{994DB8F8-3E30-433E-9C7E-D3248CBDB35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AB8CFDB-08FB-49F4-8DC6-C42992C3655C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD0DE76-69CA-488F-ADFE-BFEF1644151C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F1ED4DDD-BE62-481D-8C5C-EDABB3DC8EEC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
   <si>
     <t>diff</t>
   </si>
@@ -329,6 +329,39 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>conditions</t>
+  </si>
+  <si>
+    <t>jovenes</t>
+  </si>
+  <si>
+    <t>viejos</t>
+  </si>
+  <si>
+    <t>0.7084553</t>
+  </si>
+  <si>
+    <t>0.7088374</t>
+  </si>
+  <si>
+    <t>0.7051714</t>
+  </si>
+  <si>
+    <t>0.7049209</t>
+  </si>
+  <si>
+    <t>0.6875117</t>
+  </si>
+  <si>
+    <t>0.6855257</t>
+  </si>
+  <si>
+    <t>0.6936630</t>
+  </si>
+  <si>
+    <t>0.6953303</t>
   </si>
 </sst>
 </file>
@@ -364,9 +397,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4A14EC-C33E-4EF5-87DF-8F90C2A79719}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,424 +734,523 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
+        <v>98</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
+        <v>99</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3899130</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3898030</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
+        <v>100</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3993463</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4030856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C47" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F47" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>10</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B48" t="s">
         <v>74</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C48" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>15</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B49" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C49" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B50" t="s">
         <v>83</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C50" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B51" t="s">
         <v>87</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C51" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F51" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B52" t="s">
         <v>92</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C52" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F52" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>